<commit_message>
Update export import output unit
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="gal_per_barrel">About!$A$63</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23249,7 +23249,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23263,9 +23263,8 @@
       <c r="A2" t="s">
         <v>299</v>
       </c>
-      <c r="B2">
-        <f>10^9/About!A80</f>
-        <v>947813.39449889108</v>
+      <c r="B2" s="207">
+        <v>947800000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>